<commit_message>
update evaluation code and result
</commit_message>
<xml_diff>
--- a/ontologies/Evaluation.xlsx
+++ b/ontologies/Evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SkyTrack\workspace\SkyTrack\ontologies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC59D1F-94EA-4191-ACBB-E4E4B7E3D349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECCAE6E-38FB-4F82-816C-9B60380225FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10935" yWindow="5370" windowWidth="26325" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9105" yWindow="2700" windowWidth="26325" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="34">
   <si>
     <t>VICODI</t>
   </si>
@@ -264,6 +264,9 @@
   </si>
   <si>
     <t>ABORT</t>
+  </si>
+  <si>
+    <t>EBORT</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1051,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,6 +1337,9 @@
       <c r="F7">
         <v>1.119</v>
       </c>
+      <c r="G7" t="s">
+        <v>33</v>
+      </c>
       <c r="K7" t="s">
         <v>27</v>
       </c>
@@ -1351,6 +1357,9 @@
       </c>
       <c r="P7">
         <v>409.86599999999999</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update evaluation for Stardog
</commit_message>
<xml_diff>
--- a/ontologies/Evaluation.xlsx
+++ b/ontologies/Evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SkyTrack\workspace\SkyTrack\ontologies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECCAE6E-38FB-4F82-816C-9B60380225FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC54605-FBBD-425C-96CD-8EF8C163D3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9105" yWindow="2700" windowWidth="26325" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2115" yWindow="1650" windowWidth="26325" windowHeight="15555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
   <si>
     <t>VICODI</t>
   </si>
@@ -200,45 +200,12 @@
     <t>Owlready2</t>
   </si>
   <si>
-    <t>Pellet Loading</t>
-  </si>
-  <si>
-    <t>HermiT Loading</t>
-  </si>
-  <si>
-    <t>HermiT Validate</t>
-  </si>
-  <si>
-    <t>Jfact Loading</t>
-  </si>
-  <si>
-    <t>Pellet Validate</t>
-  </si>
-  <si>
-    <t>Jfact Validate</t>
-  </si>
-  <si>
     <t>Pellet</t>
   </si>
   <si>
     <t>HermiT</t>
   </si>
   <si>
-    <t>Jfact</t>
-  </si>
-  <si>
-    <t>Pellet - Owlready</t>
-  </si>
-  <si>
-    <t>HermiT - Owlready</t>
-  </si>
-  <si>
-    <t>Konclude Loading</t>
-  </si>
-  <si>
-    <t>Konclude Validate</t>
-  </si>
-  <si>
     <t>Konclude</t>
   </si>
   <si>
@@ -267,6 +234,9 @@
   </si>
   <si>
     <t>EBORT</t>
+  </si>
+  <si>
+    <t>Stardog</t>
   </si>
 </sst>
 </file>
@@ -335,10 +305,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -604,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B20"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,279 +732,25 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>1.1100000000000001</v>
+        <v>1.1559999999999999</v>
       </c>
       <c r="C5">
-        <v>0.127</v>
+        <v>0.107</v>
       </c>
       <c r="D5">
-        <v>0.86399999999999999</v>
+        <v>2.4889999999999999</v>
       </c>
       <c r="E5">
-        <v>1483.9110000000001</v>
+        <v>13.372</v>
       </c>
       <c r="F5">
-        <v>3.8260000000000001</v>
+        <v>40.219000000000001</v>
       </c>
       <c r="G5">
-        <v>403.16699999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>0.41099999999999998</v>
-      </c>
-      <c r="C6">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="D6">
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="E6">
-        <v>3.3719999999999999</v>
-      </c>
-      <c r="F6">
-        <v>0.60899999999999999</v>
-      </c>
-      <c r="G6">
-        <v>8.5909999999999993</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>0.64</v>
-      </c>
-      <c r="C7">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="D7">
-        <v>2.2130000000000001</v>
-      </c>
-      <c r="E7">
-        <v>9.0760000000000005</v>
-      </c>
-      <c r="F7">
-        <v>11.484</v>
-      </c>
-      <c r="G7">
-        <v>36.109000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="C8">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="D8">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="E8">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="F8">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="G8">
-        <v>55.970999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>0.38700000000000001</v>
-      </c>
-      <c r="C9">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="D9">
-        <v>0.11600000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>22.472000000000001</v>
-      </c>
-      <c r="C10">
-        <v>0.40600000000000003</v>
-      </c>
-      <c r="D10">
-        <v>1281.885</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>3.569</v>
-      </c>
-      <c r="C11">
-        <v>3.7530000000000001</v>
-      </c>
-      <c r="D11">
-        <v>5.6660000000000004</v>
-      </c>
-      <c r="E11">
-        <v>15.77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C12">
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="D12">
-        <v>2.8E-3</v>
-      </c>
-      <c r="E12">
-        <v>2.5999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <f>SUM(B5:B6)</f>
-        <v>1.5210000000000001</v>
-      </c>
-      <c r="C16">
-        <f t="shared" ref="C16:G16" si="0">SUM(C5:C6)</f>
-        <v>0.47099999999999997</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>1.3280000000000001</v>
-      </c>
-      <c r="E16">
-        <f>SUM(E5:E6)</f>
-        <v>1487.2830000000001</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>4.4350000000000005</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="0"/>
-        <v>411.75799999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <f>SUM(B7:B8)</f>
-        <v>1.3149999999999999</v>
-      </c>
-      <c r="C17">
-        <f t="shared" ref="C17:G17" si="1">SUM(C7:C8)</f>
-        <v>0.19799999999999998</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="1"/>
-        <v>2.2134</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>9.0790000000000006</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>11.484400000000001</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="1"/>
-        <v>92.08</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <f>SUM(B9:B10)</f>
-        <v>22.859000000000002</v>
-      </c>
-      <c r="C18">
-        <f t="shared" ref="C18:G18" si="2">SUM(C9:C10)</f>
-        <v>0.42100000000000004</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="2"/>
-        <v>1282.001</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19">
-        <v>5.0819999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <v>12.675000000000001</v>
+        <v>47.317999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +763,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,7 +812,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>1.1100000000000001</v>
@@ -1121,7 +833,7 @@
         <v>403.16699999999997</v>
       </c>
       <c r="K2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="L2">
         <v>0.41099999999999998</v>
@@ -1144,7 +856,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>0.64</v>
@@ -1165,7 +877,7 @@
         <v>36.109000000000002</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="L3">
         <v>0.67500000000000004</v>
@@ -1188,7 +900,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B4">
         <v>4.0000000000000001E-3</v>
@@ -1209,7 +921,7 @@
         <v>2.7149999999999999</v>
       </c>
       <c r="K4" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="L4">
         <v>0.39900000000000002</v>
@@ -1232,7 +944,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>3.569</v>
@@ -1247,13 +959,13 @@
         <v>15.77</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="L5">
         <v>3.0000000000000001E-3</v>
@@ -1268,15 +980,15 @@
         <v>2.5999999999999999E-3</v>
       </c>
       <c r="P5" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B6">
         <v>0.51600000000000001</v>
@@ -1288,16 +1000,16 @@
         <v>0.25600000000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="G6">
         <v>48.201000000000001</v>
       </c>
       <c r="K6" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="L6">
         <v>0.47599999999999998</v>
@@ -1309,10 +1021,10 @@
         <v>39.494999999999997</v>
       </c>
       <c r="O6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="P6" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q6">
         <v>219.42099999999999</v>
@@ -1320,7 +1032,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>0.38700000000000001</v>
@@ -1332,16 +1044,16 @@
         <v>0.11600000000000001</v>
       </c>
       <c r="E7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F7">
         <v>1.119</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="L7">
         <v>22.472000000000001</v>
@@ -1353,24 +1065,24 @@
         <v>1281.885</v>
       </c>
       <c r="O7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="P7">
         <v>409.86599999999999</v>
       </c>
       <c r="Q7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>5.0819999999999999</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1379,7 +1091,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>12.675000000000001</v>

</xml_diff>